<commit_message>
Updated solution for part 1 to make it prettier
</commit_message>
<xml_diff>
--- a/Day2/AoC24-Day2.xlsx
+++ b/Day2/AoC24-Day2.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Documents/GitHub Projects/AoC2024/Day1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Documents/GitHub Projects/AoC2024/Day2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E33F4265-81AD-9E41-A280-1B56C477F151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747B4CDE-5AB2-944C-9EDF-E38F46A9A2C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1780" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{47FADB5B-7636-E041-8185-C8F8E9609CF1}"/>
+    <workbookView xWindow="4380" yWindow="680" windowWidth="24420" windowHeight="16480" activeTab="1" xr2:uid="{47FADB5B-7636-E041-8185-C8F8E9609CF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 2 Part 1 Test" sheetId="1" r:id="rId1"/>
     <sheet name="Day 2 Part 1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,10 +34,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -451,7 +447,7 @@
         <v>-1</v>
       </c>
       <c r="O1" t="str">
-        <f t="shared" ref="N1:P1" si="0">(IF(NOT(ISBLANK(G1)),G1-F1,""))</f>
+        <f t="shared" ref="O1:P1" si="0">(IF(NOT(ISBLANK(G1)),G1-F1,""))</f>
         <v/>
       </c>
       <c r="P1" t="str">
@@ -793,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5CC999-7539-F34B-881C-B27E1558B08C}">
   <dimension ref="A1:V1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="T1" sqref="T1:T1000"/>
     </sheetView>
   </sheetViews>
@@ -861,7 +857,15 @@
         <v>DIFFERENT</v>
       </c>
       <c r="T1" t="str">
-        <f>IF(AND(OR(NOT(ISNUMBER(K1)),AND(K1&gt;=1,K1&lt;=3),AND(K1&lt;=-1,K1&gt;=-3)),OR(NOT(ISNUMBER(L1)),AND(L1&gt;=1,L1&lt;=3),AND(L1&lt;=-1,L1&gt;=-3)),OR(NOT(ISNUMBER(M1)),AND(M1&gt;=1,M1&lt;=3),AND(M1&lt;=-1,M1&gt;=-3)),OR(NOT(ISNUMBER(N1)),AND(N1&gt;=1,N1&lt;=3),AND(N1&lt;=-1,N1&gt;=-3)),OR(NOT(ISNUMBER(O1)),AND(O1&gt;=1,O1&lt;=3),AND(O1&lt;=-1,O1&gt;=-3)),OR(NOT(ISNUMBER(P1)),AND(P1&gt;=1,P1&lt;=3),AND(P1&lt;=-1,P1&gt;=-3)),OR(NOT(ISNUMBER(Q1)),AND(Q1&gt;=1,Q1&lt;=3),AND(Q1&lt;=-1,Q1&gt;=-3))),"SMALL","LARGE")</f>
+        <f>IF(AND(
+    IF(OR(NOT(ISNUMBER(K1)), AND(K1&lt;&gt;0, K1&gt;=-3, K1&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L1)), AND(L1&lt;&gt;0, L1&gt;=-3, L1&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M1)), AND(M1&lt;&gt;0, M1&gt;=-3, M1&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N1)), AND(N1&lt;&gt;0, N1&gt;=-3, N1&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O1)), AND(O1&lt;&gt;0, O1&gt;=-3, O1&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P1)), AND(P1&lt;&gt;0, P1&gt;=-3, P1&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q1)), AND(Q1&lt;&gt;0, Q1&gt;=-3, Q1&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>SMALL</v>
       </c>
       <c r="U1" t="str">
@@ -935,7 +939,15 @@
         <v>DIFFERENT</v>
       </c>
       <c r="T2" t="str">
-        <f t="shared" ref="T2:T65" si="10">IF(AND(OR(NOT(ISNUMBER(K2)),AND(K2&gt;=1,K2&lt;=3),AND(K2&lt;=-1,K2&gt;=-3)),OR(NOT(ISNUMBER(L2)),AND(L2&gt;=1,L2&lt;=3),AND(L2&lt;=-1,L2&gt;=-3)),OR(NOT(ISNUMBER(M2)),AND(M2&gt;=1,M2&lt;=3),AND(M2&lt;=-1,M2&gt;=-3)),OR(NOT(ISNUMBER(N2)),AND(N2&gt;=1,N2&lt;=3),AND(N2&lt;=-1,N2&gt;=-3)),OR(NOT(ISNUMBER(O2)),AND(O2&gt;=1,O2&lt;=3),AND(O2&lt;=-1,O2&gt;=-3)),OR(NOT(ISNUMBER(P2)),AND(P2&gt;=1,P2&lt;=3),AND(P2&lt;=-1,P2&gt;=-3)),OR(NOT(ISNUMBER(Q2)),AND(Q2&gt;=1,Q2&lt;=3),AND(Q2&lt;=-1,Q2&gt;=-3))),"SMALL","LARGE")</f>
+        <f t="shared" ref="T2:T65" si="10">IF(AND(
+    IF(OR(NOT(ISNUMBER(K2)), AND(K2&lt;&gt;0, K2&gt;=-3, K2&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L2)), AND(L2&lt;&gt;0, L2&gt;=-3, L2&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M2)), AND(M2&lt;&gt;0, M2&gt;=-3, M2&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N2)), AND(N2&lt;&gt;0, N2&gt;=-3, N2&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O2)), AND(O2&lt;&gt;0, O2&gt;=-3, O2&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P2)), AND(P2&lt;&gt;0, P2&gt;=-3, P2&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q2)), AND(Q2&lt;&gt;0, Q2&gt;=-3, Q2&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>LARGE</v>
       </c>
       <c r="U2" t="str">
@@ -5148,7 +5160,15 @@
         <v>DIFFERENT</v>
       </c>
       <c r="T66" t="str">
-        <f t="shared" ref="T66:T129" si="21">IF(AND(OR(NOT(ISNUMBER(K66)),AND(K66&gt;=1,K66&lt;=3),AND(K66&lt;=-1,K66&gt;=-3)),OR(NOT(ISNUMBER(L66)),AND(L66&gt;=1,L66&lt;=3),AND(L66&lt;=-1,L66&gt;=-3)),OR(NOT(ISNUMBER(M66)),AND(M66&gt;=1,M66&lt;=3),AND(M66&lt;=-1,M66&gt;=-3)),OR(NOT(ISNUMBER(N66)),AND(N66&gt;=1,N66&lt;=3),AND(N66&lt;=-1,N66&gt;=-3)),OR(NOT(ISNUMBER(O66)),AND(O66&gt;=1,O66&lt;=3),AND(O66&lt;=-1,O66&gt;=-3)),OR(NOT(ISNUMBER(P66)),AND(P66&gt;=1,P66&lt;=3),AND(P66&lt;=-1,P66&gt;=-3)),OR(NOT(ISNUMBER(Q66)),AND(Q66&gt;=1,Q66&lt;=3),AND(Q66&lt;=-1,Q66&gt;=-3))),"SMALL","LARGE")</f>
+        <f t="shared" ref="T66:T129" si="21">IF(AND(
+    IF(OR(NOT(ISNUMBER(K66)), AND(K66&lt;&gt;0, K66&gt;=-3, K66&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L66)), AND(L66&lt;&gt;0, L66&gt;=-3, L66&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M66)), AND(M66&lt;&gt;0, M66&gt;=-3, M66&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N66)), AND(N66&lt;&gt;0, N66&gt;=-3, N66&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O66)), AND(O66&lt;&gt;0, O66&gt;=-3, O66&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P66)), AND(P66&lt;&gt;0, P66&gt;=-3, P66&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q66)), AND(Q66&lt;&gt;0, Q66&gt;=-3, Q66&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>LARGE</v>
       </c>
       <c r="U66" t="str">
@@ -9364,7 +9384,15 @@
         <v>DIFFERENT</v>
       </c>
       <c r="T130" t="str">
-        <f t="shared" ref="T130:T193" si="32">IF(AND(OR(NOT(ISNUMBER(K130)),AND(K130&gt;=1,K130&lt;=3),AND(K130&lt;=-1,K130&gt;=-3)),OR(NOT(ISNUMBER(L130)),AND(L130&gt;=1,L130&lt;=3),AND(L130&lt;=-1,L130&gt;=-3)),OR(NOT(ISNUMBER(M130)),AND(M130&gt;=1,M130&lt;=3),AND(M130&lt;=-1,M130&gt;=-3)),OR(NOT(ISNUMBER(N130)),AND(N130&gt;=1,N130&lt;=3),AND(N130&lt;=-1,N130&gt;=-3)),OR(NOT(ISNUMBER(O130)),AND(O130&gt;=1,O130&lt;=3),AND(O130&lt;=-1,O130&gt;=-3)),OR(NOT(ISNUMBER(P130)),AND(P130&gt;=1,P130&lt;=3),AND(P130&lt;=-1,P130&gt;=-3)),OR(NOT(ISNUMBER(Q130)),AND(Q130&gt;=1,Q130&lt;=3),AND(Q130&lt;=-1,Q130&gt;=-3))),"SMALL","LARGE")</f>
+        <f t="shared" ref="T130:T193" si="32">IF(AND(
+    IF(OR(NOT(ISNUMBER(K130)), AND(K130&lt;&gt;0, K130&gt;=-3, K130&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L130)), AND(L130&lt;&gt;0, L130&gt;=-3, L130&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M130)), AND(M130&lt;&gt;0, M130&gt;=-3, M130&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N130)), AND(N130&lt;&gt;0, N130&gt;=-3, N130&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O130)), AND(O130&lt;&gt;0, O130&gt;=-3, O130&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P130)), AND(P130&lt;&gt;0, P130&gt;=-3, P130&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q130)), AND(Q130&lt;&gt;0, Q130&gt;=-3, Q130&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>SMALL</v>
       </c>
       <c r="U130" t="str">
@@ -13553,7 +13581,15 @@
         <v>DIFFERENT</v>
       </c>
       <c r="T194" t="str">
-        <f t="shared" ref="T194:T257" si="43">IF(AND(OR(NOT(ISNUMBER(K194)),AND(K194&gt;=1,K194&lt;=3),AND(K194&lt;=-1,K194&gt;=-3)),OR(NOT(ISNUMBER(L194)),AND(L194&gt;=1,L194&lt;=3),AND(L194&lt;=-1,L194&gt;=-3)),OR(NOT(ISNUMBER(M194)),AND(M194&gt;=1,M194&lt;=3),AND(M194&lt;=-1,M194&gt;=-3)),OR(NOT(ISNUMBER(N194)),AND(N194&gt;=1,N194&lt;=3),AND(N194&lt;=-1,N194&gt;=-3)),OR(NOT(ISNUMBER(O194)),AND(O194&gt;=1,O194&lt;=3),AND(O194&lt;=-1,O194&gt;=-3)),OR(NOT(ISNUMBER(P194)),AND(P194&gt;=1,P194&lt;=3),AND(P194&lt;=-1,P194&gt;=-3)),OR(NOT(ISNUMBER(Q194)),AND(Q194&gt;=1,Q194&lt;=3),AND(Q194&lt;=-1,Q194&gt;=-3))),"SMALL","LARGE")</f>
+        <f t="shared" ref="T194:T257" si="43">IF(AND(
+    IF(OR(NOT(ISNUMBER(K194)), AND(K194&lt;&gt;0, K194&gt;=-3, K194&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L194)), AND(L194&lt;&gt;0, L194&gt;=-3, L194&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M194)), AND(M194&lt;&gt;0, M194&gt;=-3, M194&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N194)), AND(N194&lt;&gt;0, N194&gt;=-3, N194&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O194)), AND(O194&lt;&gt;0, O194&gt;=-3, O194&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P194)), AND(P194&lt;&gt;0, P194&gt;=-3, P194&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q194)), AND(Q194&lt;&gt;0, Q194&gt;=-3, Q194&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>LARGE</v>
       </c>
       <c r="U194" t="str">
@@ -17748,7 +17784,15 @@
         <v>DIFFERENT</v>
       </c>
       <c r="T258" t="str">
-        <f t="shared" ref="T258:T321" si="54">IF(AND(OR(NOT(ISNUMBER(K258)),AND(K258&gt;=1,K258&lt;=3),AND(K258&lt;=-1,K258&gt;=-3)),OR(NOT(ISNUMBER(L258)),AND(L258&gt;=1,L258&lt;=3),AND(L258&lt;=-1,L258&gt;=-3)),OR(NOT(ISNUMBER(M258)),AND(M258&gt;=1,M258&lt;=3),AND(M258&lt;=-1,M258&gt;=-3)),OR(NOT(ISNUMBER(N258)),AND(N258&gt;=1,N258&lt;=3),AND(N258&lt;=-1,N258&gt;=-3)),OR(NOT(ISNUMBER(O258)),AND(O258&gt;=1,O258&lt;=3),AND(O258&lt;=-1,O258&gt;=-3)),OR(NOT(ISNUMBER(P258)),AND(P258&gt;=1,P258&lt;=3),AND(P258&lt;=-1,P258&gt;=-3)),OR(NOT(ISNUMBER(Q258)),AND(Q258&gt;=1,Q258&lt;=3),AND(Q258&lt;=-1,Q258&gt;=-3))),"SMALL","LARGE")</f>
+        <f t="shared" ref="T258:T321" si="54">IF(AND(
+    IF(OR(NOT(ISNUMBER(K258)), AND(K258&lt;&gt;0, K258&gt;=-3, K258&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L258)), AND(L258&lt;&gt;0, L258&gt;=-3, L258&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M258)), AND(M258&lt;&gt;0, M258&gt;=-3, M258&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N258)), AND(N258&lt;&gt;0, N258&gt;=-3, N258&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O258)), AND(O258&lt;&gt;0, O258&gt;=-3, O258&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P258)), AND(P258&lt;&gt;0, P258&gt;=-3, P258&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q258)), AND(Q258&lt;&gt;0, Q258&gt;=-3, Q258&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>LARGE</v>
       </c>
       <c r="U258" t="str">
@@ -21952,7 +21996,15 @@
         <v>DIFFERENT</v>
       </c>
       <c r="T322" t="str">
-        <f t="shared" ref="T322:T385" si="65">IF(AND(OR(NOT(ISNUMBER(K322)),AND(K322&gt;=1,K322&lt;=3),AND(K322&lt;=-1,K322&gt;=-3)),OR(NOT(ISNUMBER(L322)),AND(L322&gt;=1,L322&lt;=3),AND(L322&lt;=-1,L322&gt;=-3)),OR(NOT(ISNUMBER(M322)),AND(M322&gt;=1,M322&lt;=3),AND(M322&lt;=-1,M322&gt;=-3)),OR(NOT(ISNUMBER(N322)),AND(N322&gt;=1,N322&lt;=3),AND(N322&lt;=-1,N322&gt;=-3)),OR(NOT(ISNUMBER(O322)),AND(O322&gt;=1,O322&lt;=3),AND(O322&lt;=-1,O322&gt;=-3)),OR(NOT(ISNUMBER(P322)),AND(P322&gt;=1,P322&lt;=3),AND(P322&lt;=-1,P322&gt;=-3)),OR(NOT(ISNUMBER(Q322)),AND(Q322&gt;=1,Q322&lt;=3),AND(Q322&lt;=-1,Q322&gt;=-3))),"SMALL","LARGE")</f>
+        <f t="shared" ref="T322:T385" si="65">IF(AND(
+    IF(OR(NOT(ISNUMBER(K322)), AND(K322&lt;&gt;0, K322&gt;=-3, K322&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L322)), AND(L322&lt;&gt;0, L322&gt;=-3, L322&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M322)), AND(M322&lt;&gt;0, M322&gt;=-3, M322&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N322)), AND(N322&lt;&gt;0, N322&gt;=-3, N322&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O322)), AND(O322&lt;&gt;0, O322&gt;=-3, O322&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P322)), AND(P322&lt;&gt;0, P322&gt;=-3, P322&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q322)), AND(Q322&lt;&gt;0, Q322&gt;=-3, Q322&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>LARGE</v>
       </c>
       <c r="U322" t="str">
@@ -26165,7 +26217,15 @@
         <v>SAME</v>
       </c>
       <c r="T386" t="str">
-        <f t="shared" ref="T386:T449" si="76">IF(AND(OR(NOT(ISNUMBER(K386)),AND(K386&gt;=1,K386&lt;=3),AND(K386&lt;=-1,K386&gt;=-3)),OR(NOT(ISNUMBER(L386)),AND(L386&gt;=1,L386&lt;=3),AND(L386&lt;=-1,L386&gt;=-3)),OR(NOT(ISNUMBER(M386)),AND(M386&gt;=1,M386&lt;=3),AND(M386&lt;=-1,M386&gt;=-3)),OR(NOT(ISNUMBER(N386)),AND(N386&gt;=1,N386&lt;=3),AND(N386&lt;=-1,N386&gt;=-3)),OR(NOT(ISNUMBER(O386)),AND(O386&gt;=1,O386&lt;=3),AND(O386&lt;=-1,O386&gt;=-3)),OR(NOT(ISNUMBER(P386)),AND(P386&gt;=1,P386&lt;=3),AND(P386&lt;=-1,P386&gt;=-3)),OR(NOT(ISNUMBER(Q386)),AND(Q386&gt;=1,Q386&lt;=3),AND(Q386&lt;=-1,Q386&gt;=-3))),"SMALL","LARGE")</f>
+        <f t="shared" ref="T386:T449" si="76">IF(AND(
+    IF(OR(NOT(ISNUMBER(K386)), AND(K386&lt;&gt;0, K386&gt;=-3, K386&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L386)), AND(L386&lt;&gt;0, L386&gt;=-3, L386&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M386)), AND(M386&lt;&gt;0, M386&gt;=-3, M386&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N386)), AND(N386&lt;&gt;0, N386&gt;=-3, N386&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O386)), AND(O386&lt;&gt;0, O386&gt;=-3, O386&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P386)), AND(P386&lt;&gt;0, P386&gt;=-3, P386&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q386)), AND(Q386&lt;&gt;0, Q386&gt;=-3, Q386&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>SMALL</v>
       </c>
       <c r="U386" t="str">
@@ -30315,7 +30375,15 @@
         <v>SAME</v>
       </c>
       <c r="T450" t="str">
-        <f t="shared" ref="T450:T513" si="87">IF(AND(OR(NOT(ISNUMBER(K450)),AND(K450&gt;=1,K450&lt;=3),AND(K450&lt;=-1,K450&gt;=-3)),OR(NOT(ISNUMBER(L450)),AND(L450&gt;=1,L450&lt;=3),AND(L450&lt;=-1,L450&gt;=-3)),OR(NOT(ISNUMBER(M450)),AND(M450&gt;=1,M450&lt;=3),AND(M450&lt;=-1,M450&gt;=-3)),OR(NOT(ISNUMBER(N450)),AND(N450&gt;=1,N450&lt;=3),AND(N450&lt;=-1,N450&gt;=-3)),OR(NOT(ISNUMBER(O450)),AND(O450&gt;=1,O450&lt;=3),AND(O450&lt;=-1,O450&gt;=-3)),OR(NOT(ISNUMBER(P450)),AND(P450&gt;=1,P450&lt;=3),AND(P450&lt;=-1,P450&gt;=-3)),OR(NOT(ISNUMBER(Q450)),AND(Q450&gt;=1,Q450&lt;=3),AND(Q450&lt;=-1,Q450&gt;=-3))),"SMALL","LARGE")</f>
+        <f t="shared" ref="T450:T513" si="87">IF(AND(
+    IF(OR(NOT(ISNUMBER(K450)), AND(K450&lt;&gt;0, K450&gt;=-3, K450&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L450)), AND(L450&lt;&gt;0, L450&gt;=-3, L450&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M450)), AND(M450&lt;&gt;0, M450&gt;=-3, M450&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N450)), AND(N450&lt;&gt;0, N450&gt;=-3, N450&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O450)), AND(O450&lt;&gt;0, O450&gt;=-3, O450&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P450)), AND(P450&lt;&gt;0, P450&gt;=-3, P450&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q450)), AND(Q450&lt;&gt;0, Q450&gt;=-3, Q450&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>SMALL</v>
       </c>
       <c r="U450" t="str">
@@ -34516,7 +34584,15 @@
         <v>SAME</v>
       </c>
       <c r="T514" t="str">
-        <f t="shared" ref="T514:T577" si="98">IF(AND(OR(NOT(ISNUMBER(K514)),AND(K514&gt;=1,K514&lt;=3),AND(K514&lt;=-1,K514&gt;=-3)),OR(NOT(ISNUMBER(L514)),AND(L514&gt;=1,L514&lt;=3),AND(L514&lt;=-1,L514&gt;=-3)),OR(NOT(ISNUMBER(M514)),AND(M514&gt;=1,M514&lt;=3),AND(M514&lt;=-1,M514&gt;=-3)),OR(NOT(ISNUMBER(N514)),AND(N514&gt;=1,N514&lt;=3),AND(N514&lt;=-1,N514&gt;=-3)),OR(NOT(ISNUMBER(O514)),AND(O514&gt;=1,O514&lt;=3),AND(O514&lt;=-1,O514&gt;=-3)),OR(NOT(ISNUMBER(P514)),AND(P514&gt;=1,P514&lt;=3),AND(P514&lt;=-1,P514&gt;=-3)),OR(NOT(ISNUMBER(Q514)),AND(Q514&gt;=1,Q514&lt;=3),AND(Q514&lt;=-1,Q514&gt;=-3))),"SMALL","LARGE")</f>
+        <f t="shared" ref="T514:T577" si="98">IF(AND(
+    IF(OR(NOT(ISNUMBER(K514)), AND(K514&lt;&gt;0, K514&gt;=-3, K514&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L514)), AND(L514&lt;&gt;0, L514&gt;=-3, L514&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M514)), AND(M514&lt;&gt;0, M514&gt;=-3, M514&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N514)), AND(N514&lt;&gt;0, N514&gt;=-3, N514&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O514)), AND(O514&lt;&gt;0, O514&gt;=-3, O514&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P514)), AND(P514&lt;&gt;0, P514&gt;=-3, P514&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q514)), AND(Q514&lt;&gt;0, Q514&gt;=-3, Q514&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>SMALL</v>
       </c>
       <c r="U514" t="str">
@@ -38681,7 +38757,15 @@
         <v>SAME</v>
       </c>
       <c r="T578" t="str">
-        <f t="shared" ref="T578:T641" si="109">IF(AND(OR(NOT(ISNUMBER(K578)),AND(K578&gt;=1,K578&lt;=3),AND(K578&lt;=-1,K578&gt;=-3)),OR(NOT(ISNUMBER(L578)),AND(L578&gt;=1,L578&lt;=3),AND(L578&lt;=-1,L578&gt;=-3)),OR(NOT(ISNUMBER(M578)),AND(M578&gt;=1,M578&lt;=3),AND(M578&lt;=-1,M578&gt;=-3)),OR(NOT(ISNUMBER(N578)),AND(N578&gt;=1,N578&lt;=3),AND(N578&lt;=-1,N578&gt;=-3)),OR(NOT(ISNUMBER(O578)),AND(O578&gt;=1,O578&lt;=3),AND(O578&lt;=-1,O578&gt;=-3)),OR(NOT(ISNUMBER(P578)),AND(P578&gt;=1,P578&lt;=3),AND(P578&lt;=-1,P578&gt;=-3)),OR(NOT(ISNUMBER(Q578)),AND(Q578&gt;=1,Q578&lt;=3),AND(Q578&lt;=-1,Q578&gt;=-3))),"SMALL","LARGE")</f>
+        <f t="shared" ref="T578:T641" si="109">IF(AND(
+    IF(OR(NOT(ISNUMBER(K578)), AND(K578&lt;&gt;0, K578&gt;=-3, K578&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L578)), AND(L578&lt;&gt;0, L578&gt;=-3, L578&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M578)), AND(M578&lt;&gt;0, M578&gt;=-3, M578&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N578)), AND(N578&lt;&gt;0, N578&gt;=-3, N578&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O578)), AND(O578&lt;&gt;0, O578&gt;=-3, O578&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P578)), AND(P578&lt;&gt;0, P578&gt;=-3, P578&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q578)), AND(Q578&lt;&gt;0, Q578&gt;=-3, Q578&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>SMALL</v>
       </c>
       <c r="U578" t="str">
@@ -42918,7 +43002,15 @@
         <v>SAME</v>
       </c>
       <c r="T642" t="str">
-        <f t="shared" ref="T642:T705" si="120">IF(AND(OR(NOT(ISNUMBER(K642)),AND(K642&gt;=1,K642&lt;=3),AND(K642&lt;=-1,K642&gt;=-3)),OR(NOT(ISNUMBER(L642)),AND(L642&gt;=1,L642&lt;=3),AND(L642&lt;=-1,L642&gt;=-3)),OR(NOT(ISNUMBER(M642)),AND(M642&gt;=1,M642&lt;=3),AND(M642&lt;=-1,M642&gt;=-3)),OR(NOT(ISNUMBER(N642)),AND(N642&gt;=1,N642&lt;=3),AND(N642&lt;=-1,N642&gt;=-3)),OR(NOT(ISNUMBER(O642)),AND(O642&gt;=1,O642&lt;=3),AND(O642&lt;=-1,O642&gt;=-3)),OR(NOT(ISNUMBER(P642)),AND(P642&gt;=1,P642&lt;=3),AND(P642&lt;=-1,P642&gt;=-3)),OR(NOT(ISNUMBER(Q642)),AND(Q642&gt;=1,Q642&lt;=3),AND(Q642&lt;=-1,Q642&gt;=-3))),"SMALL","LARGE")</f>
+        <f t="shared" ref="T642:T705" si="120">IF(AND(
+    IF(OR(NOT(ISNUMBER(K642)), AND(K642&lt;&gt;0, K642&gt;=-3, K642&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L642)), AND(L642&lt;&gt;0, L642&gt;=-3, L642&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M642)), AND(M642&lt;&gt;0, M642&gt;=-3, M642&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N642)), AND(N642&lt;&gt;0, N642&gt;=-3, N642&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O642)), AND(O642&lt;&gt;0, O642&gt;=-3, O642&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P642)), AND(P642&lt;&gt;0, P642&gt;=-3, P642&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q642)), AND(Q642&lt;&gt;0, Q642&gt;=-3, Q642&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>SMALL</v>
       </c>
       <c r="U642" t="str">
@@ -47080,7 +47172,15 @@
         <v>SAME</v>
       </c>
       <c r="T706" t="str">
-        <f t="shared" ref="T706:T769" si="131">IF(AND(OR(NOT(ISNUMBER(K706)),AND(K706&gt;=1,K706&lt;=3),AND(K706&lt;=-1,K706&gt;=-3)),OR(NOT(ISNUMBER(L706)),AND(L706&gt;=1,L706&lt;=3),AND(L706&lt;=-1,L706&gt;=-3)),OR(NOT(ISNUMBER(M706)),AND(M706&gt;=1,M706&lt;=3),AND(M706&lt;=-1,M706&gt;=-3)),OR(NOT(ISNUMBER(N706)),AND(N706&gt;=1,N706&lt;=3),AND(N706&lt;=-1,N706&gt;=-3)),OR(NOT(ISNUMBER(O706)),AND(O706&gt;=1,O706&lt;=3),AND(O706&lt;=-1,O706&gt;=-3)),OR(NOT(ISNUMBER(P706)),AND(P706&gt;=1,P706&lt;=3),AND(P706&lt;=-1,P706&gt;=-3)),OR(NOT(ISNUMBER(Q706)),AND(Q706&gt;=1,Q706&lt;=3),AND(Q706&lt;=-1,Q706&gt;=-3))),"SMALL","LARGE")</f>
+        <f t="shared" ref="T706:T769" si="131">IF(AND(
+    IF(OR(NOT(ISNUMBER(K706)), AND(K706&lt;&gt;0, K706&gt;=-3, K706&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L706)), AND(L706&lt;&gt;0, L706&gt;=-3, L706&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M706)), AND(M706&lt;&gt;0, M706&gt;=-3, M706&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N706)), AND(N706&lt;&gt;0, N706&gt;=-3, N706&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O706)), AND(O706&lt;&gt;0, O706&gt;=-3, O706&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P706)), AND(P706&lt;&gt;0, P706&gt;=-3, P706&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q706)), AND(Q706&lt;&gt;0, Q706&gt;=-3, Q706&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>SMALL</v>
       </c>
       <c r="U706" t="str">
@@ -51326,7 +51426,15 @@
         <v>SAME</v>
       </c>
       <c r="T770" t="str">
-        <f t="shared" ref="T770:T833" si="142">IF(AND(OR(NOT(ISNUMBER(K770)),AND(K770&gt;=1,K770&lt;=3),AND(K770&lt;=-1,K770&gt;=-3)),OR(NOT(ISNUMBER(L770)),AND(L770&gt;=1,L770&lt;=3),AND(L770&lt;=-1,L770&gt;=-3)),OR(NOT(ISNUMBER(M770)),AND(M770&gt;=1,M770&lt;=3),AND(M770&lt;=-1,M770&gt;=-3)),OR(NOT(ISNUMBER(N770)),AND(N770&gt;=1,N770&lt;=3),AND(N770&lt;=-1,N770&gt;=-3)),OR(NOT(ISNUMBER(O770)),AND(O770&gt;=1,O770&lt;=3),AND(O770&lt;=-1,O770&gt;=-3)),OR(NOT(ISNUMBER(P770)),AND(P770&gt;=1,P770&lt;=3),AND(P770&lt;=-1,P770&gt;=-3)),OR(NOT(ISNUMBER(Q770)),AND(Q770&gt;=1,Q770&lt;=3),AND(Q770&lt;=-1,Q770&gt;=-3))),"SMALL","LARGE")</f>
+        <f t="shared" ref="T770:T833" si="142">IF(AND(
+    IF(OR(NOT(ISNUMBER(K770)), AND(K770&lt;&gt;0, K770&gt;=-3, K770&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L770)), AND(L770&lt;&gt;0, L770&gt;=-3, L770&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M770)), AND(M770&lt;&gt;0, M770&gt;=-3, M770&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N770)), AND(N770&lt;&gt;0, N770&gt;=-3, N770&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O770)), AND(O770&lt;&gt;0, O770&gt;=-3, O770&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P770)), AND(P770&lt;&gt;0, P770&gt;=-3, P770&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q770)), AND(Q770&lt;&gt;0, Q770&gt;=-3, Q770&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>SMALL</v>
       </c>
       <c r="U770" t="str">
@@ -55509,7 +55617,15 @@
         <v>SAME</v>
       </c>
       <c r="T834" t="str">
-        <f t="shared" ref="T834:T897" si="153">IF(AND(OR(NOT(ISNUMBER(K834)),AND(K834&gt;=1,K834&lt;=3),AND(K834&lt;=-1,K834&gt;=-3)),OR(NOT(ISNUMBER(L834)),AND(L834&gt;=1,L834&lt;=3),AND(L834&lt;=-1,L834&gt;=-3)),OR(NOT(ISNUMBER(M834)),AND(M834&gt;=1,M834&lt;=3),AND(M834&lt;=-1,M834&gt;=-3)),OR(NOT(ISNUMBER(N834)),AND(N834&gt;=1,N834&lt;=3),AND(N834&lt;=-1,N834&gt;=-3)),OR(NOT(ISNUMBER(O834)),AND(O834&gt;=1,O834&lt;=3),AND(O834&lt;=-1,O834&gt;=-3)),OR(NOT(ISNUMBER(P834)),AND(P834&gt;=1,P834&lt;=3),AND(P834&lt;=-1,P834&gt;=-3)),OR(NOT(ISNUMBER(Q834)),AND(Q834&gt;=1,Q834&lt;=3),AND(Q834&lt;=-1,Q834&gt;=-3))),"SMALL","LARGE")</f>
+        <f t="shared" ref="T834:T897" si="153">IF(AND(
+    IF(OR(NOT(ISNUMBER(K834)), AND(K834&lt;&gt;0, K834&gt;=-3, K834&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L834)), AND(L834&lt;&gt;0, L834&gt;=-3, L834&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M834)), AND(M834&lt;&gt;0, M834&gt;=-3, M834&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N834)), AND(N834&lt;&gt;0, N834&gt;=-3, N834&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O834)), AND(O834&lt;&gt;0, O834&gt;=-3, O834&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P834)), AND(P834&lt;&gt;0, P834&gt;=-3, P834&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q834)), AND(Q834&lt;&gt;0, Q834&gt;=-3, Q834&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>SMALL</v>
       </c>
       <c r="U834" t="str">
@@ -59704,7 +59820,15 @@
         <v>SAME</v>
       </c>
       <c r="T898" t="str">
-        <f t="shared" ref="T898:T961" si="164">IF(AND(OR(NOT(ISNUMBER(K898)),AND(K898&gt;=1,K898&lt;=3),AND(K898&lt;=-1,K898&gt;=-3)),OR(NOT(ISNUMBER(L898)),AND(L898&gt;=1,L898&lt;=3),AND(L898&lt;=-1,L898&gt;=-3)),OR(NOT(ISNUMBER(M898)),AND(M898&gt;=1,M898&lt;=3),AND(M898&lt;=-1,M898&gt;=-3)),OR(NOT(ISNUMBER(N898)),AND(N898&gt;=1,N898&lt;=3),AND(N898&lt;=-1,N898&gt;=-3)),OR(NOT(ISNUMBER(O898)),AND(O898&gt;=1,O898&lt;=3),AND(O898&lt;=-1,O898&gt;=-3)),OR(NOT(ISNUMBER(P898)),AND(P898&gt;=1,P898&lt;=3),AND(P898&lt;=-1,P898&gt;=-3)),OR(NOT(ISNUMBER(Q898)),AND(Q898&gt;=1,Q898&lt;=3),AND(Q898&lt;=-1,Q898&gt;=-3))),"SMALL","LARGE")</f>
+        <f t="shared" ref="T898:T961" si="164">IF(AND(
+    IF(OR(NOT(ISNUMBER(K898)), AND(K898&lt;&gt;0, K898&gt;=-3, K898&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L898)), AND(L898&lt;&gt;0, L898&gt;=-3, L898&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M898)), AND(M898&lt;&gt;0, M898&gt;=-3, M898&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N898)), AND(N898&lt;&gt;0, N898&gt;=-3, N898&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O898)), AND(O898&lt;&gt;0, O898&gt;=-3, O898&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P898)), AND(P898&lt;&gt;0, P898&gt;=-3, P898&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q898)), AND(Q898&lt;&gt;0, Q898&gt;=-3, Q898&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>SMALL</v>
       </c>
       <c r="U898" t="str">
@@ -63863,7 +63987,15 @@
         <v>SAME</v>
       </c>
       <c r="T962" t="str">
-        <f t="shared" ref="T962:T1000" si="175">IF(AND(OR(NOT(ISNUMBER(K962)),AND(K962&gt;=1,K962&lt;=3),AND(K962&lt;=-1,K962&gt;=-3)),OR(NOT(ISNUMBER(L962)),AND(L962&gt;=1,L962&lt;=3),AND(L962&lt;=-1,L962&gt;=-3)),OR(NOT(ISNUMBER(M962)),AND(M962&gt;=1,M962&lt;=3),AND(M962&lt;=-1,M962&gt;=-3)),OR(NOT(ISNUMBER(N962)),AND(N962&gt;=1,N962&lt;=3),AND(N962&lt;=-1,N962&gt;=-3)),OR(NOT(ISNUMBER(O962)),AND(O962&gt;=1,O962&lt;=3),AND(O962&lt;=-1,O962&gt;=-3)),OR(NOT(ISNUMBER(P962)),AND(P962&gt;=1,P962&lt;=3),AND(P962&lt;=-1,P962&gt;=-3)),OR(NOT(ISNUMBER(Q962)),AND(Q962&gt;=1,Q962&lt;=3),AND(Q962&lt;=-1,Q962&gt;=-3))),"SMALL","LARGE")</f>
+        <f t="shared" ref="T962:T1000" si="175">IF(AND(
+    IF(OR(NOT(ISNUMBER(K962)), AND(K962&lt;&gt;0, K962&gt;=-3, K962&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(L962)), AND(L962&lt;&gt;0, L962&gt;=-3, L962&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(M962)), AND(M962&lt;&gt;0, M962&gt;=-3, M962&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(N962)), AND(N962&lt;&gt;0, N962&gt;=-3, N962&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(O962)), AND(O962&lt;&gt;0, O962&gt;=-3, O962&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(P962)), AND(P962&lt;&gt;0, P962&gt;=-3, P962&lt;=3)), TRUE, FALSE),
+    IF(OR(NOT(ISNUMBER(Q962)), AND(Q962&lt;&gt;0, Q962&gt;=-3, Q962&lt;=3)), TRUE, FALSE)
+), "SMALL", "LARGE")</f>
         <v>SMALL</v>
       </c>
       <c r="U962" t="str">

</xml_diff>